<commit_message>
update after paper acceptance
</commit_message>
<xml_diff>
--- a/src/stat/stats.xlsx
+++ b/src/stat/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\GitHub\PhD\topography-control-of-ice-albedo\src\stat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35498827-28A9-4D67-9448-C644ABB6727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE2B6DA-558E-475E-B06D-0F68B5D9F842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="1620" windowWidth="18225" windowHeight="11385" activeTab="3" xr2:uid="{ABE177B4-A381-4848-9D74-5AD89FAA9339}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{ABE177B4-A381-4848-9D74-5AD89FAA9339}"/>
   </bookViews>
   <sheets>
     <sheet name="SW" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -164,8 +167,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -255,12 +258,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,6 +274,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF6A4A18"/>
+      <color rgb="FF29416A"/>
+      <color rgb="FFBDC5E6"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFACC5FF"/>
+      <color rgb="FF31414A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -319,7 +332,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="29416A"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -340,13 +353,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-DK"/>
@@ -430,7 +443,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="BDC5E6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -451,13 +464,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-DK"/>
@@ -582,16 +595,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-DK"/>
@@ -642,16 +655,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-DK"/>
@@ -689,7 +702,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1100"/>
+        <a:defRPr sz="1600">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-DK"/>
     </a:p>
@@ -739,7 +755,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="6A4A18"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -760,13 +776,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-DK"/>
@@ -850,7 +866,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="ACC5FF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -871,13 +887,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-DK"/>
@@ -1002,16 +1018,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-DK"/>
@@ -1062,16 +1078,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-DK"/>
@@ -1109,7 +1125,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1100"/>
+        <a:defRPr sz="1600">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-DK"/>
     </a:p>
@@ -2239,16 +2258,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>331470</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>453390</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>55245</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>148590</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2623,36 +2642,36 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="15"/>
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="13"/>
+      <c r="L1" s="15"/>
       <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13" t="s">
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="13"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2967,14 +2986,14 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="13"/>
+      <c r="H1" s="15"/>
       <c r="L1" s="8" t="s">
         <v>15</v>
       </c>
@@ -3445,14 +3464,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -3567,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9643780-4F75-4F93-9184-D7F7A8A52441}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3610,13 +3629,13 @@
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>0</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>0</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3628,13 +3647,13 @@
       <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>0</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>0</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3646,13 +3665,13 @@
       <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>6.6436710125683599E-147</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>3.3078515089393401E-20</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>6.43528188297059E-37</v>
       </c>
     </row>
@@ -3664,13 +3683,13 @@
       <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>8.6239249435440596E-252</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>9.9133630952210404E-76</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>6.6997662026060902E-66</v>
       </c>
     </row>
@@ -3682,13 +3701,13 @@
       <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>1.2447537332816E-9</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0.99990733285681799</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>0.82363632498527195</v>
       </c>
     </row>
@@ -3700,13 +3719,13 @@
       <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>1.2447537332816E-9</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>4.4703892925809797E-16</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>1.4549880194122199E-14</v>
       </c>
     </row>
@@ -3720,13 +3739,13 @@
       <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>3.4324688170019998E-101</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>3.4324688170019998E-101</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>2.1870323943237401E-79</v>
       </c>
     </row>
@@ -3738,13 +3757,13 @@
       <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>8.1629793963890896E-32</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>6.0516780081415596E-31</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <v>5.6286513645771299E-49</v>
       </c>
     </row>
@@ -3756,13 +3775,13 @@
       <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>3.8326118912055998E-7</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>8.3024013664644804E-13</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <v>4.3981401728895403E-8</v>
       </c>
     </row>
@@ -3774,13 +3793,13 @@
       <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>7.4885853171620095E-46</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>3.4915466533238098E-34</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <v>2.9629588627984402E-28</v>
       </c>
     </row>
@@ -3792,13 +3811,13 @@
       <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>5.1663718684869402E-13</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>6.4166269186979302E-3</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>2.3818607697825999E-4</v>
       </c>
     </row>
@@ -3810,13 +3829,13 @@
       <c r="C14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>0.99999999999948297</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>3.8497040340020599E-22</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>5.6327139432714899E-13</v>
       </c>
     </row>
@@ -3830,13 +3849,13 @@
       <c r="C15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>6.4930772428296299E-39</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>6.4930772428296299E-39</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>1.1901036083549699E-32</v>
       </c>
     </row>
@@ -3848,13 +3867,13 @@
       <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>2.8433073733934198E-209</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>3.2670372229328398E-51</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>7.26972874405016E-61</v>
       </c>
     </row>
@@ -3866,13 +3885,13 @@
       <c r="C17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>1</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>1</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>1</v>
       </c>
     </row>
@@ -3884,13 +3903,13 @@
       <c r="C18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>1</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <v>0.999999999999999</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>0.99999991033241498</v>
       </c>
     </row>
@@ -3902,13 +3921,13 @@
       <c r="C19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>0</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <v>5.2810902498381996E-47</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <v>6.2727281702898397E-18</v>
       </c>
     </row>
@@ -3920,13 +3939,13 @@
       <c r="C20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="14">
         <v>1</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="14">
         <v>0.27207838816583502</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <v>0.88940439310286901</v>
       </c>
     </row>
@@ -3940,13 +3959,13 @@
       <c r="C21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>0</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>0</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3958,13 +3977,13 @@
       <c r="C22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="14">
         <v>0</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="14">
         <v>0</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3976,13 +3995,13 @@
       <c r="C23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="14">
         <v>0</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="14">
         <v>1.09384381106953E-89</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <v>7.3114961388608203E-152</v>
       </c>
     </row>
@@ -3994,13 +4013,13 @@
       <c r="C24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="14">
         <v>2.8387073312257002E-300</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="14">
         <v>3.78644789286627E-26</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <v>7.4926128295268899E-11</v>
       </c>
     </row>
@@ -4016,8 +4035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AD66C2-5A8C-4967-8316-5B78E5CD59C3}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4061,19 +4080,19 @@
       <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>0.218</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <v>0.375</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="13">
         <f>0.252</f>
         <v>0.252</v>
       </c>
@@ -4089,22 +4108,22 @@
       <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <f>1-G2</f>
         <v>0.76400000000000001</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <f>1-H2</f>
         <v>0.78200000000000003</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <f>1-K2</f>
         <v>0.625</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="13">
         <f>1-L2</f>
         <v>0.748</v>
       </c>
@@ -4150,7 +4169,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>